<commit_message>
Add strategic recommendations to vendor spreadsheet
- Added new column "Strategic Recommendation" to Excel file
- Implemented strict classification rules:
  * Terminate (78): Hotels, restaurants, catering, events, travel, non-critical services
  * Consolidate (263): Overlapping SaaS, multiple agencies, duplicate services
  * Optimize (45): Mission-critical platforms (AWS, Salesforce, Microsoft, etc.)
- Color-coded recommendations with formatting
- Created add_strategic_recommendations.py script for automation
- Total: 386 vendors analyzed and categorized
</commit_message>
<xml_diff>
--- a/Vendor Analysis Assessment - Deeba.xlsx
+++ b/Vendor Analysis Assessment - Deeba.xlsx
@@ -22,7 +22,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -71,8 +71,25 @@
       <b val="1"/>
       <color theme="1"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="000D652D"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00CC6600"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00CC0000"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -83,6 +100,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF073763"/>
         <bgColor rgb="FF073763"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00366092"/>
+        <bgColor rgb="00366092"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E6F4EA"/>
+        <bgColor rgb="00E6F4EA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF4E6"/>
+        <bgColor rgb="00FFF4E6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFE6E6"/>
+        <bgColor rgb="00FFE6E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -142,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -229,6 +270,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +557,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O814"/>
+  <dimension ref="A1:P814"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -518,6 +571,7 @@
     <col width="16.38" customWidth="1" style="33" min="3" max="3"/>
     <col width="47" customWidth="1" style="33" min="4" max="4"/>
     <col width="28.25" customWidth="1" style="33" min="5" max="5"/>
+    <col width="25" customWidth="1" style="33" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -556,6 +610,11 @@
       <c r="M1" s="6" t="n"/>
       <c r="N1" s="6" t="n"/>
       <c r="O1" s="6" t="n"/>
+      <c r="P1" s="34" t="inlineStr">
+        <is>
+          <t>Strategic Recommendation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
@@ -583,6 +642,11 @@
       <c r="M2" s="12" t="n"/>
       <c r="N2" s="12" t="n"/>
       <c r="O2" s="12" t="n"/>
+      <c r="P2" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="inlineStr">
@@ -610,6 +674,11 @@
       <c r="M3" s="12" t="n"/>
       <c r="N3" s="12" t="n"/>
       <c r="O3" s="12" t="n"/>
+      <c r="P3" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="7" t="inlineStr">
@@ -637,6 +706,11 @@
       <c r="M4" s="12" t="n"/>
       <c r="N4" s="12" t="n"/>
       <c r="O4" s="12" t="n"/>
+      <c r="P4" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="inlineStr">
@@ -664,6 +738,11 @@
       <c r="M5" s="12" t="n"/>
       <c r="N5" s="12" t="n"/>
       <c r="O5" s="12" t="n"/>
+      <c r="P5" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
@@ -691,6 +770,11 @@
       <c r="M6" s="12" t="n"/>
       <c r="N6" s="12" t="n"/>
       <c r="O6" s="12" t="n"/>
+      <c r="P6" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="inlineStr">
@@ -718,6 +802,11 @@
       <c r="M7" s="12" t="n"/>
       <c r="N7" s="12" t="n"/>
       <c r="O7" s="12" t="n"/>
+      <c r="P7" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="inlineStr">
@@ -745,6 +834,11 @@
       <c r="M8" s="12" t="n"/>
       <c r="N8" s="12" t="n"/>
       <c r="O8" s="12" t="n"/>
+      <c r="P8" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="inlineStr">
@@ -772,6 +866,11 @@
       <c r="M9" s="12" t="n"/>
       <c r="N9" s="12" t="n"/>
       <c r="O9" s="12" t="n"/>
+      <c r="P9" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
@@ -799,6 +898,11 @@
       <c r="M10" s="12" t="n"/>
       <c r="N10" s="12" t="n"/>
       <c r="O10" s="12" t="n"/>
+      <c r="P10" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="7" t="inlineStr">
@@ -826,6 +930,11 @@
       <c r="M11" s="12" t="n"/>
       <c r="N11" s="12" t="n"/>
       <c r="O11" s="12" t="n"/>
+      <c r="P11" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="7" t="inlineStr">
@@ -853,6 +962,11 @@
       <c r="M12" s="12" t="n"/>
       <c r="N12" s="12" t="n"/>
       <c r="O12" s="12" t="n"/>
+      <c r="P12" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="7" t="inlineStr">
@@ -880,6 +994,11 @@
       <c r="M13" s="12" t="n"/>
       <c r="N13" s="12" t="n"/>
       <c r="O13" s="12" t="n"/>
+      <c r="P13" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="7" t="inlineStr">
@@ -907,6 +1026,11 @@
       <c r="M14" s="12" t="n"/>
       <c r="N14" s="12" t="n"/>
       <c r="O14" s="12" t="n"/>
+      <c r="P14" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="7" t="inlineStr">
@@ -934,6 +1058,11 @@
       <c r="M15" s="12" t="n"/>
       <c r="N15" s="12" t="n"/>
       <c r="O15" s="12" t="n"/>
+      <c r="P15" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="7" t="inlineStr">
@@ -961,6 +1090,11 @@
       <c r="M16" s="12" t="n"/>
       <c r="N16" s="12" t="n"/>
       <c r="O16" s="12" t="n"/>
+      <c r="P16" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="7" t="inlineStr">
@@ -988,6 +1122,11 @@
       <c r="M17" s="12" t="n"/>
       <c r="N17" s="12" t="n"/>
       <c r="O17" s="12" t="n"/>
+      <c r="P17" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="7" t="inlineStr">
@@ -1015,6 +1154,11 @@
       <c r="M18" s="12" t="n"/>
       <c r="N18" s="12" t="n"/>
       <c r="O18" s="12" t="n"/>
+      <c r="P18" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="7" t="inlineStr">
@@ -1042,6 +1186,11 @@
       <c r="M19" s="12" t="n"/>
       <c r="N19" s="12" t="n"/>
       <c r="O19" s="12" t="n"/>
+      <c r="P19" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="7" t="inlineStr">
@@ -1069,6 +1218,11 @@
       <c r="M20" s="12" t="n"/>
       <c r="N20" s="12" t="n"/>
       <c r="O20" s="12" t="n"/>
+      <c r="P20" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="7" t="inlineStr">
@@ -1096,6 +1250,11 @@
       <c r="M21" s="12" t="n"/>
       <c r="N21" s="12" t="n"/>
       <c r="O21" s="12" t="n"/>
+      <c r="P21" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="inlineStr">
@@ -1123,6 +1282,11 @@
       <c r="M22" s="12" t="n"/>
       <c r="N22" s="12" t="n"/>
       <c r="O22" s="12" t="n"/>
+      <c r="P22" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="inlineStr">
@@ -1150,6 +1314,11 @@
       <c r="M23" s="12" t="n"/>
       <c r="N23" s="12" t="n"/>
       <c r="O23" s="12" t="n"/>
+      <c r="P23" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="inlineStr">
@@ -1177,6 +1346,11 @@
       <c r="M24" s="12" t="n"/>
       <c r="N24" s="12" t="n"/>
       <c r="O24" s="12" t="n"/>
+      <c r="P24" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="inlineStr">
@@ -1204,6 +1378,11 @@
       <c r="M25" s="12" t="n"/>
       <c r="N25" s="12" t="n"/>
       <c r="O25" s="12" t="n"/>
+      <c r="P25" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="inlineStr">
@@ -1231,6 +1410,11 @@
       <c r="M26" s="12" t="n"/>
       <c r="N26" s="12" t="n"/>
       <c r="O26" s="12" t="n"/>
+      <c r="P26" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="inlineStr">
@@ -1258,6 +1442,11 @@
       <c r="M27" s="12" t="n"/>
       <c r="N27" s="12" t="n"/>
       <c r="O27" s="12" t="n"/>
+      <c r="P27" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="inlineStr">
@@ -1285,6 +1474,11 @@
       <c r="M28" s="12" t="n"/>
       <c r="N28" s="12" t="n"/>
       <c r="O28" s="12" t="n"/>
+      <c r="P28" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="7" t="inlineStr">
@@ -1312,6 +1506,11 @@
       <c r="M29" s="12" t="n"/>
       <c r="N29" s="12" t="n"/>
       <c r="O29" s="12" t="n"/>
+      <c r="P29" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="7" t="inlineStr">
@@ -1339,6 +1538,11 @@
       <c r="M30" s="12" t="n"/>
       <c r="N30" s="12" t="n"/>
       <c r="O30" s="12" t="n"/>
+      <c r="P30" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="7" t="inlineStr">
@@ -1366,6 +1570,11 @@
       <c r="M31" s="12" t="n"/>
       <c r="N31" s="12" t="n"/>
       <c r="O31" s="12" t="n"/>
+      <c r="P31" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="7" t="inlineStr">
@@ -1393,6 +1602,11 @@
       <c r="M32" s="12" t="n"/>
       <c r="N32" s="12" t="n"/>
       <c r="O32" s="12" t="n"/>
+      <c r="P32" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="7" t="inlineStr">
@@ -1420,6 +1634,11 @@
       <c r="M33" s="12" t="n"/>
       <c r="N33" s="12" t="n"/>
       <c r="O33" s="12" t="n"/>
+      <c r="P33" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="7" t="inlineStr">
@@ -1447,6 +1666,11 @@
       <c r="M34" s="12" t="n"/>
       <c r="N34" s="12" t="n"/>
       <c r="O34" s="12" t="n"/>
+      <c r="P34" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="7" t="inlineStr">
@@ -1474,6 +1698,11 @@
       <c r="M35" s="12" t="n"/>
       <c r="N35" s="12" t="n"/>
       <c r="O35" s="12" t="n"/>
+      <c r="P35" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="7" t="inlineStr">
@@ -1501,6 +1730,11 @@
       <c r="M36" s="12" t="n"/>
       <c r="N36" s="12" t="n"/>
       <c r="O36" s="12" t="n"/>
+      <c r="P36" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="7" t="inlineStr">
@@ -1528,6 +1762,11 @@
       <c r="M37" s="12" t="n"/>
       <c r="N37" s="12" t="n"/>
       <c r="O37" s="12" t="n"/>
+      <c r="P37" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="7" t="inlineStr">
@@ -1555,6 +1794,11 @@
       <c r="M38" s="12" t="n"/>
       <c r="N38" s="12" t="n"/>
       <c r="O38" s="12" t="n"/>
+      <c r="P38" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="7" t="inlineStr">
@@ -1582,6 +1826,11 @@
       <c r="M39" s="12" t="n"/>
       <c r="N39" s="12" t="n"/>
       <c r="O39" s="12" t="n"/>
+      <c r="P39" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="7" t="inlineStr">
@@ -1609,6 +1858,11 @@
       <c r="M40" s="12" t="n"/>
       <c r="N40" s="12" t="n"/>
       <c r="O40" s="12" t="n"/>
+      <c r="P40" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="7" t="inlineStr">
@@ -1636,6 +1890,11 @@
       <c r="M41" s="12" t="n"/>
       <c r="N41" s="12" t="n"/>
       <c r="O41" s="12" t="n"/>
+      <c r="P41" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="7" t="inlineStr">
@@ -1663,6 +1922,11 @@
       <c r="M42" s="12" t="n"/>
       <c r="N42" s="12" t="n"/>
       <c r="O42" s="12" t="n"/>
+      <c r="P42" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="7" t="inlineStr">
@@ -1690,6 +1954,11 @@
       <c r="M43" s="12" t="n"/>
       <c r="N43" s="12" t="n"/>
       <c r="O43" s="12" t="n"/>
+      <c r="P43" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="7" t="inlineStr">
@@ -1717,6 +1986,11 @@
       <c r="M44" s="12" t="n"/>
       <c r="N44" s="12" t="n"/>
       <c r="O44" s="12" t="n"/>
+      <c r="P44" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="7" t="inlineStr">
@@ -1744,6 +2018,11 @@
       <c r="M45" s="12" t="n"/>
       <c r="N45" s="12" t="n"/>
       <c r="O45" s="12" t="n"/>
+      <c r="P45" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="7" t="inlineStr">
@@ -1771,6 +2050,11 @@
       <c r="M46" s="12" t="n"/>
       <c r="N46" s="12" t="n"/>
       <c r="O46" s="12" t="n"/>
+      <c r="P46" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="7" t="inlineStr">
@@ -1798,6 +2082,11 @@
       <c r="M47" s="12" t="n"/>
       <c r="N47" s="12" t="n"/>
       <c r="O47" s="12" t="n"/>
+      <c r="P47" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="7" t="inlineStr">
@@ -1825,6 +2114,11 @@
       <c r="M48" s="12" t="n"/>
       <c r="N48" s="12" t="n"/>
       <c r="O48" s="12" t="n"/>
+      <c r="P48" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="7" t="inlineStr">
@@ -1852,6 +2146,11 @@
       <c r="M49" s="12" t="n"/>
       <c r="N49" s="12" t="n"/>
       <c r="O49" s="12" t="n"/>
+      <c r="P49" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="7" t="inlineStr">
@@ -1879,6 +2178,11 @@
       <c r="M50" s="12" t="n"/>
       <c r="N50" s="12" t="n"/>
       <c r="O50" s="12" t="n"/>
+      <c r="P50" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="7" t="inlineStr">
@@ -1906,6 +2210,11 @@
       <c r="M51" s="12" t="n"/>
       <c r="N51" s="12" t="n"/>
       <c r="O51" s="12" t="n"/>
+      <c r="P51" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="7" t="inlineStr">
@@ -1933,6 +2242,11 @@
       <c r="M52" s="12" t="n"/>
       <c r="N52" s="12" t="n"/>
       <c r="O52" s="12" t="n"/>
+      <c r="P52" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="7" t="inlineStr">
@@ -1960,6 +2274,11 @@
       <c r="M53" s="12" t="n"/>
       <c r="N53" s="12" t="n"/>
       <c r="O53" s="12" t="n"/>
+      <c r="P53" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="7" t="inlineStr">
@@ -1987,6 +2306,11 @@
       <c r="M54" s="12" t="n"/>
       <c r="N54" s="12" t="n"/>
       <c r="O54" s="12" t="n"/>
+      <c r="P54" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="7" t="inlineStr">
@@ -2014,6 +2338,11 @@
       <c r="M55" s="12" t="n"/>
       <c r="N55" s="12" t="n"/>
       <c r="O55" s="12" t="n"/>
+      <c r="P55" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="7" t="inlineStr">
@@ -2041,6 +2370,11 @@
       <c r="M56" s="12" t="n"/>
       <c r="N56" s="12" t="n"/>
       <c r="O56" s="12" t="n"/>
+      <c r="P56" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="7" t="inlineStr">
@@ -2068,6 +2402,11 @@
       <c r="M57" s="12" t="n"/>
       <c r="N57" s="12" t="n"/>
       <c r="O57" s="12" t="n"/>
+      <c r="P57" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="7" t="inlineStr">
@@ -2095,6 +2434,11 @@
       <c r="M58" s="12" t="n"/>
       <c r="N58" s="12" t="n"/>
       <c r="O58" s="12" t="n"/>
+      <c r="P58" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="7" t="inlineStr">
@@ -2122,6 +2466,11 @@
       <c r="M59" s="12" t="n"/>
       <c r="N59" s="12" t="n"/>
       <c r="O59" s="12" t="n"/>
+      <c r="P59" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="7" t="inlineStr">
@@ -2149,6 +2498,11 @@
       <c r="M60" s="12" t="n"/>
       <c r="N60" s="12" t="n"/>
       <c r="O60" s="12" t="n"/>
+      <c r="P60" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="7" t="inlineStr">
@@ -2176,6 +2530,11 @@
       <c r="M61" s="12" t="n"/>
       <c r="N61" s="12" t="n"/>
       <c r="O61" s="12" t="n"/>
+      <c r="P61" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="7" t="inlineStr">
@@ -2203,6 +2562,11 @@
       <c r="M62" s="12" t="n"/>
       <c r="N62" s="12" t="n"/>
       <c r="O62" s="12" t="n"/>
+      <c r="P62" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="7" t="inlineStr">
@@ -2230,6 +2594,11 @@
       <c r="M63" s="12" t="n"/>
       <c r="N63" s="12" t="n"/>
       <c r="O63" s="12" t="n"/>
+      <c r="P63" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="7" t="inlineStr">
@@ -2257,6 +2626,11 @@
       <c r="M64" s="12" t="n"/>
       <c r="N64" s="12" t="n"/>
       <c r="O64" s="12" t="n"/>
+      <c r="P64" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="7" t="inlineStr">
@@ -2284,6 +2658,11 @@
       <c r="M65" s="12" t="n"/>
       <c r="N65" s="12" t="n"/>
       <c r="O65" s="12" t="n"/>
+      <c r="P65" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="7" t="inlineStr">
@@ -2311,6 +2690,11 @@
       <c r="M66" s="12" t="n"/>
       <c r="N66" s="12" t="n"/>
       <c r="O66" s="12" t="n"/>
+      <c r="P66" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="7" t="inlineStr">
@@ -2338,6 +2722,11 @@
       <c r="M67" s="12" t="n"/>
       <c r="N67" s="12" t="n"/>
       <c r="O67" s="12" t="n"/>
+      <c r="P67" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="7" t="inlineStr">
@@ -2365,6 +2754,11 @@
       <c r="M68" s="12" t="n"/>
       <c r="N68" s="12" t="n"/>
       <c r="O68" s="12" t="n"/>
+      <c r="P68" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="7" t="inlineStr">
@@ -2392,6 +2786,11 @@
       <c r="M69" s="12" t="n"/>
       <c r="N69" s="12" t="n"/>
       <c r="O69" s="12" t="n"/>
+      <c r="P69" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="7" t="inlineStr">
@@ -2419,6 +2818,11 @@
       <c r="M70" s="12" t="n"/>
       <c r="N70" s="12" t="n"/>
       <c r="O70" s="12" t="n"/>
+      <c r="P70" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="7" t="inlineStr">
@@ -2446,6 +2850,11 @@
       <c r="M71" s="12" t="n"/>
       <c r="N71" s="12" t="n"/>
       <c r="O71" s="12" t="n"/>
+      <c r="P71" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="7" t="inlineStr">
@@ -2473,6 +2882,11 @@
       <c r="M72" s="12" t="n"/>
       <c r="N72" s="12" t="n"/>
       <c r="O72" s="12" t="n"/>
+      <c r="P72" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="7" t="inlineStr">
@@ -2500,6 +2914,11 @@
       <c r="M73" s="12" t="n"/>
       <c r="N73" s="12" t="n"/>
       <c r="O73" s="12" t="n"/>
+      <c r="P73" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="7" t="inlineStr">
@@ -2527,6 +2946,11 @@
       <c r="M74" s="12" t="n"/>
       <c r="N74" s="12" t="n"/>
       <c r="O74" s="12" t="n"/>
+      <c r="P74" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="7" t="inlineStr">
@@ -2554,6 +2978,11 @@
       <c r="M75" s="12" t="n"/>
       <c r="N75" s="12" t="n"/>
       <c r="O75" s="12" t="n"/>
+      <c r="P75" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="7" t="inlineStr">
@@ -2581,6 +3010,11 @@
       <c r="M76" s="12" t="n"/>
       <c r="N76" s="12" t="n"/>
       <c r="O76" s="12" t="n"/>
+      <c r="P76" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="7" t="inlineStr">
@@ -2608,6 +3042,11 @@
       <c r="M77" s="12" t="n"/>
       <c r="N77" s="12" t="n"/>
       <c r="O77" s="12" t="n"/>
+      <c r="P77" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="7" t="inlineStr">
@@ -2635,6 +3074,11 @@
       <c r="M78" s="12" t="n"/>
       <c r="N78" s="12" t="n"/>
       <c r="O78" s="12" t="n"/>
+      <c r="P78" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="7" t="inlineStr">
@@ -2662,6 +3106,11 @@
       <c r="M79" s="12" t="n"/>
       <c r="N79" s="12" t="n"/>
       <c r="O79" s="12" t="n"/>
+      <c r="P79" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="7" t="inlineStr">
@@ -2689,6 +3138,11 @@
       <c r="M80" s="12" t="n"/>
       <c r="N80" s="12" t="n"/>
       <c r="O80" s="12" t="n"/>
+      <c r="P80" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="7" t="inlineStr">
@@ -2716,6 +3170,11 @@
       <c r="M81" s="12" t="n"/>
       <c r="N81" s="12" t="n"/>
       <c r="O81" s="12" t="n"/>
+      <c r="P81" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="7" t="inlineStr">
@@ -2743,6 +3202,11 @@
       <c r="M82" s="12" t="n"/>
       <c r="N82" s="12" t="n"/>
       <c r="O82" s="12" t="n"/>
+      <c r="P82" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="7" t="inlineStr">
@@ -2770,6 +3234,11 @@
       <c r="M83" s="12" t="n"/>
       <c r="N83" s="12" t="n"/>
       <c r="O83" s="12" t="n"/>
+      <c r="P83" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="7" t="inlineStr">
@@ -2797,6 +3266,11 @@
       <c r="M84" s="12" t="n"/>
       <c r="N84" s="12" t="n"/>
       <c r="O84" s="12" t="n"/>
+      <c r="P84" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="7" t="inlineStr">
@@ -2824,6 +3298,11 @@
       <c r="M85" s="12" t="n"/>
       <c r="N85" s="12" t="n"/>
       <c r="O85" s="12" t="n"/>
+      <c r="P85" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="7" t="inlineStr">
@@ -2851,6 +3330,11 @@
       <c r="M86" s="12" t="n"/>
       <c r="N86" s="12" t="n"/>
       <c r="O86" s="12" t="n"/>
+      <c r="P86" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="7" t="inlineStr">
@@ -2878,6 +3362,11 @@
       <c r="M87" s="12" t="n"/>
       <c r="N87" s="12" t="n"/>
       <c r="O87" s="12" t="n"/>
+      <c r="P87" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="7" t="inlineStr">
@@ -2905,6 +3394,11 @@
       <c r="M88" s="12" t="n"/>
       <c r="N88" s="12" t="n"/>
       <c r="O88" s="12" t="n"/>
+      <c r="P88" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="7" t="inlineStr">
@@ -2932,6 +3426,11 @@
       <c r="M89" s="12" t="n"/>
       <c r="N89" s="12" t="n"/>
       <c r="O89" s="12" t="n"/>
+      <c r="P89" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="7" t="inlineStr">
@@ -2959,6 +3458,11 @@
       <c r="M90" s="12" t="n"/>
       <c r="N90" s="12" t="n"/>
       <c r="O90" s="12" t="n"/>
+      <c r="P90" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="7" t="inlineStr">
@@ -2986,6 +3490,11 @@
       <c r="M91" s="12" t="n"/>
       <c r="N91" s="12" t="n"/>
       <c r="O91" s="12" t="n"/>
+      <c r="P91" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="7" t="inlineStr">
@@ -3013,6 +3522,11 @@
       <c r="M92" s="12" t="n"/>
       <c r="N92" s="12" t="n"/>
       <c r="O92" s="12" t="n"/>
+      <c r="P92" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="7" t="inlineStr">
@@ -3040,6 +3554,11 @@
       <c r="M93" s="12" t="n"/>
       <c r="N93" s="12" t="n"/>
       <c r="O93" s="12" t="n"/>
+      <c r="P93" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="7" t="inlineStr">
@@ -3067,6 +3586,11 @@
       <c r="M94" s="12" t="n"/>
       <c r="N94" s="12" t="n"/>
       <c r="O94" s="12" t="n"/>
+      <c r="P94" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="7" t="inlineStr">
@@ -3094,6 +3618,11 @@
       <c r="M95" s="12" t="n"/>
       <c r="N95" s="12" t="n"/>
       <c r="O95" s="12" t="n"/>
+      <c r="P95" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="7" t="inlineStr">
@@ -3121,6 +3650,11 @@
       <c r="M96" s="12" t="n"/>
       <c r="N96" s="12" t="n"/>
       <c r="O96" s="12" t="n"/>
+      <c r="P96" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="7" t="inlineStr">
@@ -3148,6 +3682,11 @@
       <c r="M97" s="12" t="n"/>
       <c r="N97" s="12" t="n"/>
       <c r="O97" s="12" t="n"/>
+      <c r="P97" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="7" t="inlineStr">
@@ -3175,6 +3714,11 @@
       <c r="M98" s="12" t="n"/>
       <c r="N98" s="12" t="n"/>
       <c r="O98" s="12" t="n"/>
+      <c r="P98" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="7" t="inlineStr">
@@ -3202,6 +3746,11 @@
       <c r="M99" s="12" t="n"/>
       <c r="N99" s="12" t="n"/>
       <c r="O99" s="12" t="n"/>
+      <c r="P99" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="7" t="inlineStr">
@@ -3229,6 +3778,11 @@
       <c r="M100" s="12" t="n"/>
       <c r="N100" s="12" t="n"/>
       <c r="O100" s="12" t="n"/>
+      <c r="P100" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="7" t="inlineStr">
@@ -3256,6 +3810,11 @@
       <c r="M101" s="12" t="n"/>
       <c r="N101" s="12" t="n"/>
       <c r="O101" s="12" t="n"/>
+      <c r="P101" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="7" t="inlineStr">
@@ -3283,6 +3842,11 @@
       <c r="M102" s="12" t="n"/>
       <c r="N102" s="12" t="n"/>
       <c r="O102" s="12" t="n"/>
+      <c r="P102" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="7" t="inlineStr">
@@ -3310,6 +3874,11 @@
       <c r="M103" s="12" t="n"/>
       <c r="N103" s="12" t="n"/>
       <c r="O103" s="12" t="n"/>
+      <c r="P103" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="7" t="inlineStr">
@@ -3337,6 +3906,11 @@
       <c r="M104" s="12" t="n"/>
       <c r="N104" s="12" t="n"/>
       <c r="O104" s="12" t="n"/>
+      <c r="P104" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="7" t="inlineStr">
@@ -3364,6 +3938,11 @@
       <c r="M105" s="12" t="n"/>
       <c r="N105" s="12" t="n"/>
       <c r="O105" s="12" t="n"/>
+      <c r="P105" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="7" t="inlineStr">
@@ -3391,6 +3970,11 @@
       <c r="M106" s="12" t="n"/>
       <c r="N106" s="12" t="n"/>
       <c r="O106" s="12" t="n"/>
+      <c r="P106" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="7" t="inlineStr">
@@ -3418,6 +4002,11 @@
       <c r="M107" s="12" t="n"/>
       <c r="N107" s="12" t="n"/>
       <c r="O107" s="12" t="n"/>
+      <c r="P107" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="7" t="inlineStr">
@@ -3445,6 +4034,11 @@
       <c r="M108" s="12" t="n"/>
       <c r="N108" s="12" t="n"/>
       <c r="O108" s="12" t="n"/>
+      <c r="P108" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="7" t="inlineStr">
@@ -3472,6 +4066,11 @@
       <c r="M109" s="12" t="n"/>
       <c r="N109" s="12" t="n"/>
       <c r="O109" s="12" t="n"/>
+      <c r="P109" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="7" t="inlineStr">
@@ -3499,6 +4098,11 @@
       <c r="M110" s="12" t="n"/>
       <c r="N110" s="12" t="n"/>
       <c r="O110" s="12" t="n"/>
+      <c r="P110" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="7" t="inlineStr">
@@ -3526,6 +4130,11 @@
       <c r="M111" s="12" t="n"/>
       <c r="N111" s="12" t="n"/>
       <c r="O111" s="12" t="n"/>
+      <c r="P111" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="7" t="inlineStr">
@@ -3553,6 +4162,11 @@
       <c r="M112" s="12" t="n"/>
       <c r="N112" s="12" t="n"/>
       <c r="O112" s="12" t="n"/>
+      <c r="P112" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="7" t="inlineStr">
@@ -3580,6 +4194,11 @@
       <c r="M113" s="12" t="n"/>
       <c r="N113" s="12" t="n"/>
       <c r="O113" s="12" t="n"/>
+      <c r="P113" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="7" t="inlineStr">
@@ -3607,6 +4226,11 @@
       <c r="M114" s="12" t="n"/>
       <c r="N114" s="12" t="n"/>
       <c r="O114" s="12" t="n"/>
+      <c r="P114" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="7" t="inlineStr">
@@ -3634,6 +4258,11 @@
       <c r="M115" s="12" t="n"/>
       <c r="N115" s="12" t="n"/>
       <c r="O115" s="12" t="n"/>
+      <c r="P115" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="7" t="inlineStr">
@@ -3661,6 +4290,11 @@
       <c r="M116" s="12" t="n"/>
       <c r="N116" s="12" t="n"/>
       <c r="O116" s="12" t="n"/>
+      <c r="P116" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="7" t="inlineStr">
@@ -3688,6 +4322,11 @@
       <c r="M117" s="12" t="n"/>
       <c r="N117" s="12" t="n"/>
       <c r="O117" s="12" t="n"/>
+      <c r="P117" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="7" t="inlineStr">
@@ -3715,6 +4354,11 @@
       <c r="M118" s="12" t="n"/>
       <c r="N118" s="12" t="n"/>
       <c r="O118" s="12" t="n"/>
+      <c r="P118" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="7" t="inlineStr">
@@ -3742,6 +4386,11 @@
       <c r="M119" s="12" t="n"/>
       <c r="N119" s="12" t="n"/>
       <c r="O119" s="12" t="n"/>
+      <c r="P119" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="7" t="inlineStr">
@@ -3769,6 +4418,11 @@
       <c r="M120" s="12" t="n"/>
       <c r="N120" s="12" t="n"/>
       <c r="O120" s="12" t="n"/>
+      <c r="P120" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="7" t="inlineStr">
@@ -3796,6 +4450,11 @@
       <c r="M121" s="12" t="n"/>
       <c r="N121" s="12" t="n"/>
       <c r="O121" s="12" t="n"/>
+      <c r="P121" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="7" t="inlineStr">
@@ -3823,6 +4482,11 @@
       <c r="M122" s="12" t="n"/>
       <c r="N122" s="12" t="n"/>
       <c r="O122" s="12" t="n"/>
+      <c r="P122" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="7" t="inlineStr">
@@ -3850,6 +4514,11 @@
       <c r="M123" s="12" t="n"/>
       <c r="N123" s="12" t="n"/>
       <c r="O123" s="12" t="n"/>
+      <c r="P123" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="7" t="inlineStr">
@@ -3877,6 +4546,11 @@
       <c r="M124" s="12" t="n"/>
       <c r="N124" s="12" t="n"/>
       <c r="O124" s="12" t="n"/>
+      <c r="P124" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="7" t="inlineStr">
@@ -3904,6 +4578,11 @@
       <c r="M125" s="12" t="n"/>
       <c r="N125" s="12" t="n"/>
       <c r="O125" s="12" t="n"/>
+      <c r="P125" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="7" t="inlineStr">
@@ -3931,6 +4610,11 @@
       <c r="M126" s="12" t="n"/>
       <c r="N126" s="12" t="n"/>
       <c r="O126" s="12" t="n"/>
+      <c r="P126" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="7" t="inlineStr">
@@ -3958,6 +4642,11 @@
       <c r="M127" s="12" t="n"/>
       <c r="N127" s="12" t="n"/>
       <c r="O127" s="12" t="n"/>
+      <c r="P127" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="7" t="inlineStr">
@@ -3985,6 +4674,11 @@
       <c r="M128" s="12" t="n"/>
       <c r="N128" s="12" t="n"/>
       <c r="O128" s="12" t="n"/>
+      <c r="P128" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="7" t="inlineStr">
@@ -4012,6 +4706,11 @@
       <c r="M129" s="12" t="n"/>
       <c r="N129" s="12" t="n"/>
       <c r="O129" s="12" t="n"/>
+      <c r="P129" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="7" t="inlineStr">
@@ -4039,6 +4738,11 @@
       <c r="M130" s="12" t="n"/>
       <c r="N130" s="12" t="n"/>
       <c r="O130" s="12" t="n"/>
+      <c r="P130" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="7" t="inlineStr">
@@ -4066,6 +4770,11 @@
       <c r="M131" s="12" t="n"/>
       <c r="N131" s="12" t="n"/>
       <c r="O131" s="12" t="n"/>
+      <c r="P131" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="7" t="inlineStr">
@@ -4093,6 +4802,11 @@
       <c r="M132" s="12" t="n"/>
       <c r="N132" s="12" t="n"/>
       <c r="O132" s="12" t="n"/>
+      <c r="P132" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="7" t="inlineStr">
@@ -4120,6 +4834,11 @@
       <c r="M133" s="12" t="n"/>
       <c r="N133" s="12" t="n"/>
       <c r="O133" s="12" t="n"/>
+      <c r="P133" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="7" t="inlineStr">
@@ -4147,6 +4866,11 @@
       <c r="M134" s="12" t="n"/>
       <c r="N134" s="12" t="n"/>
       <c r="O134" s="12" t="n"/>
+      <c r="P134" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="7" t="inlineStr">
@@ -4174,6 +4898,11 @@
       <c r="M135" s="12" t="n"/>
       <c r="N135" s="12" t="n"/>
       <c r="O135" s="12" t="n"/>
+      <c r="P135" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="7" t="inlineStr">
@@ -4201,6 +4930,11 @@
       <c r="M136" s="12" t="n"/>
       <c r="N136" s="12" t="n"/>
       <c r="O136" s="12" t="n"/>
+      <c r="P136" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="7" t="inlineStr">
@@ -4228,6 +4962,11 @@
       <c r="M137" s="12" t="n"/>
       <c r="N137" s="12" t="n"/>
       <c r="O137" s="12" t="n"/>
+      <c r="P137" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="7" t="inlineStr">
@@ -4255,6 +4994,11 @@
       <c r="M138" s="12" t="n"/>
       <c r="N138" s="12" t="n"/>
       <c r="O138" s="12" t="n"/>
+      <c r="P138" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="7" t="inlineStr">
@@ -4282,6 +5026,11 @@
       <c r="M139" s="12" t="n"/>
       <c r="N139" s="12" t="n"/>
       <c r="O139" s="12" t="n"/>
+      <c r="P139" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="7" t="inlineStr">
@@ -4309,6 +5058,11 @@
       <c r="M140" s="12" t="n"/>
       <c r="N140" s="12" t="n"/>
       <c r="O140" s="12" t="n"/>
+      <c r="P140" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="7" t="inlineStr">
@@ -4336,6 +5090,11 @@
       <c r="M141" s="12" t="n"/>
       <c r="N141" s="12" t="n"/>
       <c r="O141" s="12" t="n"/>
+      <c r="P141" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="7" t="inlineStr">
@@ -4363,6 +5122,11 @@
       <c r="M142" s="12" t="n"/>
       <c r="N142" s="12" t="n"/>
       <c r="O142" s="12" t="n"/>
+      <c r="P142" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="7" t="inlineStr">
@@ -4390,6 +5154,11 @@
       <c r="M143" s="12" t="n"/>
       <c r="N143" s="12" t="n"/>
       <c r="O143" s="12" t="n"/>
+      <c r="P143" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="7" t="inlineStr">
@@ -4417,6 +5186,11 @@
       <c r="M144" s="12" t="n"/>
       <c r="N144" s="12" t="n"/>
       <c r="O144" s="12" t="n"/>
+      <c r="P144" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="7" t="inlineStr">
@@ -4444,6 +5218,11 @@
       <c r="M145" s="12" t="n"/>
       <c r="N145" s="12" t="n"/>
       <c r="O145" s="12" t="n"/>
+      <c r="P145" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="7" t="inlineStr">
@@ -4471,6 +5250,11 @@
       <c r="M146" s="12" t="n"/>
       <c r="N146" s="12" t="n"/>
       <c r="O146" s="12" t="n"/>
+      <c r="P146" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="7" t="inlineStr">
@@ -4498,6 +5282,11 @@
       <c r="M147" s="12" t="n"/>
       <c r="N147" s="12" t="n"/>
       <c r="O147" s="12" t="n"/>
+      <c r="P147" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="7" t="inlineStr">
@@ -4525,6 +5314,11 @@
       <c r="M148" s="12" t="n"/>
       <c r="N148" s="12" t="n"/>
       <c r="O148" s="12" t="n"/>
+      <c r="P148" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="7" t="inlineStr">
@@ -4552,6 +5346,11 @@
       <c r="M149" s="12" t="n"/>
       <c r="N149" s="12" t="n"/>
       <c r="O149" s="12" t="n"/>
+      <c r="P149" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="7" t="inlineStr">
@@ -4579,6 +5378,11 @@
       <c r="M150" s="12" t="n"/>
       <c r="N150" s="12" t="n"/>
       <c r="O150" s="12" t="n"/>
+      <c r="P150" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="7" t="inlineStr">
@@ -4606,6 +5410,11 @@
       <c r="M151" s="12" t="n"/>
       <c r="N151" s="12" t="n"/>
       <c r="O151" s="12" t="n"/>
+      <c r="P151" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="7" t="inlineStr">
@@ -4633,6 +5442,11 @@
       <c r="M152" s="12" t="n"/>
       <c r="N152" s="12" t="n"/>
       <c r="O152" s="12" t="n"/>
+      <c r="P152" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="7" t="inlineStr">
@@ -4660,6 +5474,11 @@
       <c r="M153" s="12" t="n"/>
       <c r="N153" s="12" t="n"/>
       <c r="O153" s="12" t="n"/>
+      <c r="P153" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="7" t="inlineStr">
@@ -4687,6 +5506,11 @@
       <c r="M154" s="12" t="n"/>
       <c r="N154" s="12" t="n"/>
       <c r="O154" s="12" t="n"/>
+      <c r="P154" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="7" t="inlineStr">
@@ -4714,6 +5538,11 @@
       <c r="M155" s="12" t="n"/>
       <c r="N155" s="12" t="n"/>
       <c r="O155" s="12" t="n"/>
+      <c r="P155" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="7" t="inlineStr">
@@ -4741,6 +5570,11 @@
       <c r="M156" s="12" t="n"/>
       <c r="N156" s="12" t="n"/>
       <c r="O156" s="12" t="n"/>
+      <c r="P156" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="7" t="inlineStr">
@@ -4768,6 +5602,11 @@
       <c r="M157" s="12" t="n"/>
       <c r="N157" s="12" t="n"/>
       <c r="O157" s="12" t="n"/>
+      <c r="P157" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="7" t="inlineStr">
@@ -4795,6 +5634,11 @@
       <c r="M158" s="12" t="n"/>
       <c r="N158" s="12" t="n"/>
       <c r="O158" s="12" t="n"/>
+      <c r="P158" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="7" t="inlineStr">
@@ -4822,6 +5666,11 @@
       <c r="M159" s="12" t="n"/>
       <c r="N159" s="12" t="n"/>
       <c r="O159" s="12" t="n"/>
+      <c r="P159" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="7" t="inlineStr">
@@ -4849,6 +5698,11 @@
       <c r="M160" s="12" t="n"/>
       <c r="N160" s="12" t="n"/>
       <c r="O160" s="12" t="n"/>
+      <c r="P160" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="7" t="inlineStr">
@@ -4876,6 +5730,11 @@
       <c r="M161" s="12" t="n"/>
       <c r="N161" s="12" t="n"/>
       <c r="O161" s="12" t="n"/>
+      <c r="P161" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="7" t="inlineStr">
@@ -4903,6 +5762,11 @@
       <c r="M162" s="12" t="n"/>
       <c r="N162" s="12" t="n"/>
       <c r="O162" s="12" t="n"/>
+      <c r="P162" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="7" t="inlineStr">
@@ -4930,6 +5794,11 @@
       <c r="M163" s="12" t="n"/>
       <c r="N163" s="12" t="n"/>
       <c r="O163" s="12" t="n"/>
+      <c r="P163" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="7" t="inlineStr">
@@ -4957,6 +5826,11 @@
       <c r="M164" s="12" t="n"/>
       <c r="N164" s="12" t="n"/>
       <c r="O164" s="12" t="n"/>
+      <c r="P164" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="7" t="inlineStr">
@@ -4984,6 +5858,11 @@
       <c r="M165" s="12" t="n"/>
       <c r="N165" s="12" t="n"/>
       <c r="O165" s="12" t="n"/>
+      <c r="P165" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="7" t="inlineStr">
@@ -5011,6 +5890,11 @@
       <c r="M166" s="12" t="n"/>
       <c r="N166" s="12" t="n"/>
       <c r="O166" s="12" t="n"/>
+      <c r="P166" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="7" t="inlineStr">
@@ -5038,6 +5922,11 @@
       <c r="M167" s="12" t="n"/>
       <c r="N167" s="12" t="n"/>
       <c r="O167" s="12" t="n"/>
+      <c r="P167" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="7" t="inlineStr">
@@ -5065,6 +5954,11 @@
       <c r="M168" s="12" t="n"/>
       <c r="N168" s="12" t="n"/>
       <c r="O168" s="12" t="n"/>
+      <c r="P168" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="7" t="inlineStr">
@@ -5092,6 +5986,11 @@
       <c r="M169" s="12" t="n"/>
       <c r="N169" s="12" t="n"/>
       <c r="O169" s="12" t="n"/>
+      <c r="P169" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="7" t="inlineStr">
@@ -5119,6 +6018,11 @@
       <c r="M170" s="12" t="n"/>
       <c r="N170" s="12" t="n"/>
       <c r="O170" s="12" t="n"/>
+      <c r="P170" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="7" t="inlineStr">
@@ -5146,6 +6050,11 @@
       <c r="M171" s="12" t="n"/>
       <c r="N171" s="12" t="n"/>
       <c r="O171" s="12" t="n"/>
+      <c r="P171" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="7" t="inlineStr">
@@ -5173,6 +6082,11 @@
       <c r="M172" s="12" t="n"/>
       <c r="N172" s="12" t="n"/>
       <c r="O172" s="12" t="n"/>
+      <c r="P172" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="7" t="inlineStr">
@@ -5200,6 +6114,11 @@
       <c r="M173" s="12" t="n"/>
       <c r="N173" s="12" t="n"/>
       <c r="O173" s="12" t="n"/>
+      <c r="P173" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="7" t="inlineStr">
@@ -5227,6 +6146,11 @@
       <c r="M174" s="12" t="n"/>
       <c r="N174" s="12" t="n"/>
       <c r="O174" s="12" t="n"/>
+      <c r="P174" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="7" t="inlineStr">
@@ -5254,6 +6178,11 @@
       <c r="M175" s="12" t="n"/>
       <c r="N175" s="12" t="n"/>
       <c r="O175" s="12" t="n"/>
+      <c r="P175" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="7" t="inlineStr">
@@ -5281,6 +6210,11 @@
       <c r="M176" s="12" t="n"/>
       <c r="N176" s="12" t="n"/>
       <c r="O176" s="12" t="n"/>
+      <c r="P176" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="7" t="inlineStr">
@@ -5308,6 +6242,11 @@
       <c r="M177" s="12" t="n"/>
       <c r="N177" s="12" t="n"/>
       <c r="O177" s="12" t="n"/>
+      <c r="P177" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="7" t="inlineStr">
@@ -5335,6 +6274,11 @@
       <c r="M178" s="12" t="n"/>
       <c r="N178" s="12" t="n"/>
       <c r="O178" s="12" t="n"/>
+      <c r="P178" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="7" t="inlineStr">
@@ -5362,6 +6306,11 @@
       <c r="M179" s="12" t="n"/>
       <c r="N179" s="12" t="n"/>
       <c r="O179" s="12" t="n"/>
+      <c r="P179" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="7" t="inlineStr">
@@ -5389,6 +6338,11 @@
       <c r="M180" s="12" t="n"/>
       <c r="N180" s="12" t="n"/>
       <c r="O180" s="12" t="n"/>
+      <c r="P180" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="7" t="inlineStr">
@@ -5416,6 +6370,11 @@
       <c r="M181" s="12" t="n"/>
       <c r="N181" s="12" t="n"/>
       <c r="O181" s="12" t="n"/>
+      <c r="P181" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="7" t="inlineStr">
@@ -5443,6 +6402,11 @@
       <c r="M182" s="12" t="n"/>
       <c r="N182" s="12" t="n"/>
       <c r="O182" s="12" t="n"/>
+      <c r="P182" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="7" t="inlineStr">
@@ -5470,6 +6434,11 @@
       <c r="M183" s="12" t="n"/>
       <c r="N183" s="12" t="n"/>
       <c r="O183" s="12" t="n"/>
+      <c r="P183" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="7" t="inlineStr">
@@ -5497,6 +6466,11 @@
       <c r="M184" s="12" t="n"/>
       <c r="N184" s="12" t="n"/>
       <c r="O184" s="12" t="n"/>
+      <c r="P184" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="7" t="inlineStr">
@@ -5524,6 +6498,11 @@
       <c r="M185" s="12" t="n"/>
       <c r="N185" s="12" t="n"/>
       <c r="O185" s="12" t="n"/>
+      <c r="P185" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="7" t="inlineStr">
@@ -5551,6 +6530,11 @@
       <c r="M186" s="12" t="n"/>
       <c r="N186" s="12" t="n"/>
       <c r="O186" s="12" t="n"/>
+      <c r="P186" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="7" t="inlineStr">
@@ -5578,6 +6562,11 @@
       <c r="M187" s="12" t="n"/>
       <c r="N187" s="12" t="n"/>
       <c r="O187" s="12" t="n"/>
+      <c r="P187" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="7" t="inlineStr">
@@ -5605,6 +6594,11 @@
       <c r="M188" s="12" t="n"/>
       <c r="N188" s="12" t="n"/>
       <c r="O188" s="12" t="n"/>
+      <c r="P188" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="7" t="inlineStr">
@@ -5632,6 +6626,11 @@
       <c r="M189" s="12" t="n"/>
       <c r="N189" s="12" t="n"/>
       <c r="O189" s="12" t="n"/>
+      <c r="P189" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="7" t="inlineStr">
@@ -5659,6 +6658,11 @@
       <c r="M190" s="12" t="n"/>
       <c r="N190" s="12" t="n"/>
       <c r="O190" s="12" t="n"/>
+      <c r="P190" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="7" t="inlineStr">
@@ -5686,6 +6690,11 @@
       <c r="M191" s="12" t="n"/>
       <c r="N191" s="12" t="n"/>
       <c r="O191" s="12" t="n"/>
+      <c r="P191" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="7" t="inlineStr">
@@ -5713,6 +6722,11 @@
       <c r="M192" s="12" t="n"/>
       <c r="N192" s="12" t="n"/>
       <c r="O192" s="12" t="n"/>
+      <c r="P192" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="7" t="inlineStr">
@@ -5740,6 +6754,11 @@
       <c r="M193" s="12" t="n"/>
       <c r="N193" s="12" t="n"/>
       <c r="O193" s="12" t="n"/>
+      <c r="P193" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="7" t="inlineStr">
@@ -5767,6 +6786,11 @@
       <c r="M194" s="12" t="n"/>
       <c r="N194" s="12" t="n"/>
       <c r="O194" s="12" t="n"/>
+      <c r="P194" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="7" t="inlineStr">
@@ -5794,6 +6818,11 @@
       <c r="M195" s="12" t="n"/>
       <c r="N195" s="12" t="n"/>
       <c r="O195" s="12" t="n"/>
+      <c r="P195" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="7" t="inlineStr">
@@ -5821,6 +6850,11 @@
       <c r="M196" s="12" t="n"/>
       <c r="N196" s="12" t="n"/>
       <c r="O196" s="12" t="n"/>
+      <c r="P196" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="7" t="inlineStr">
@@ -5848,6 +6882,11 @@
       <c r="M197" s="12" t="n"/>
       <c r="N197" s="12" t="n"/>
       <c r="O197" s="12" t="n"/>
+      <c r="P197" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="7" t="inlineStr">
@@ -5875,6 +6914,11 @@
       <c r="M198" s="12" t="n"/>
       <c r="N198" s="12" t="n"/>
       <c r="O198" s="12" t="n"/>
+      <c r="P198" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="7" t="inlineStr">
@@ -5902,6 +6946,11 @@
       <c r="M199" s="12" t="n"/>
       <c r="N199" s="12" t="n"/>
       <c r="O199" s="12" t="n"/>
+      <c r="P199" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="7" t="inlineStr">
@@ -5929,6 +6978,11 @@
       <c r="M200" s="12" t="n"/>
       <c r="N200" s="12" t="n"/>
       <c r="O200" s="12" t="n"/>
+      <c r="P200" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="7" t="inlineStr">
@@ -5956,6 +7010,11 @@
       <c r="M201" s="12" t="n"/>
       <c r="N201" s="12" t="n"/>
       <c r="O201" s="12" t="n"/>
+      <c r="P201" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="7" t="inlineStr">
@@ -5983,6 +7042,11 @@
       <c r="M202" s="12" t="n"/>
       <c r="N202" s="12" t="n"/>
       <c r="O202" s="12" t="n"/>
+      <c r="P202" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="14" t="inlineStr">
@@ -6010,6 +7074,11 @@
       <c r="M203" s="12" t="n"/>
       <c r="N203" s="12" t="n"/>
       <c r="O203" s="12" t="n"/>
+      <c r="P203" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="7" t="inlineStr">
@@ -6037,6 +7106,11 @@
       <c r="M204" s="12" t="n"/>
       <c r="N204" s="12" t="n"/>
       <c r="O204" s="12" t="n"/>
+      <c r="P204" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="7" t="inlineStr">
@@ -6064,6 +7138,11 @@
       <c r="M205" s="12" t="n"/>
       <c r="N205" s="12" t="n"/>
       <c r="O205" s="12" t="n"/>
+      <c r="P205" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="7" t="inlineStr">
@@ -6091,6 +7170,11 @@
       <c r="M206" s="12" t="n"/>
       <c r="N206" s="12" t="n"/>
       <c r="O206" s="12" t="n"/>
+      <c r="P206" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="7" t="inlineStr">
@@ -6118,6 +7202,11 @@
       <c r="M207" s="12" t="n"/>
       <c r="N207" s="12" t="n"/>
       <c r="O207" s="12" t="n"/>
+      <c r="P207" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="7" t="inlineStr">
@@ -6145,6 +7234,11 @@
       <c r="M208" s="12" t="n"/>
       <c r="N208" s="12" t="n"/>
       <c r="O208" s="12" t="n"/>
+      <c r="P208" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="7" t="inlineStr">
@@ -6172,6 +7266,11 @@
       <c r="M209" s="12" t="n"/>
       <c r="N209" s="12" t="n"/>
       <c r="O209" s="12" t="n"/>
+      <c r="P209" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="7" t="inlineStr">
@@ -6199,6 +7298,11 @@
       <c r="M210" s="12" t="n"/>
       <c r="N210" s="12" t="n"/>
       <c r="O210" s="12" t="n"/>
+      <c r="P210" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="7" t="inlineStr">
@@ -6226,6 +7330,11 @@
       <c r="M211" s="12" t="n"/>
       <c r="N211" s="12" t="n"/>
       <c r="O211" s="12" t="n"/>
+      <c r="P211" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="7" t="inlineStr">
@@ -6253,6 +7362,11 @@
       <c r="M212" s="12" t="n"/>
       <c r="N212" s="12" t="n"/>
       <c r="O212" s="12" t="n"/>
+      <c r="P212" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="7" t="inlineStr">
@@ -6280,6 +7394,11 @@
       <c r="M213" s="12" t="n"/>
       <c r="N213" s="12" t="n"/>
       <c r="O213" s="12" t="n"/>
+      <c r="P213" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="7" t="inlineStr">
@@ -6307,6 +7426,11 @@
       <c r="M214" s="12" t="n"/>
       <c r="N214" s="12" t="n"/>
       <c r="O214" s="12" t="n"/>
+      <c r="P214" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="7" t="inlineStr">
@@ -6334,6 +7458,11 @@
       <c r="M215" s="12" t="n"/>
       <c r="N215" s="12" t="n"/>
       <c r="O215" s="12" t="n"/>
+      <c r="P215" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="7" t="inlineStr">
@@ -6361,6 +7490,11 @@
       <c r="M216" s="12" t="n"/>
       <c r="N216" s="12" t="n"/>
       <c r="O216" s="12" t="n"/>
+      <c r="P216" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="7" t="inlineStr">
@@ -6388,6 +7522,11 @@
       <c r="M217" s="12" t="n"/>
       <c r="N217" s="12" t="n"/>
       <c r="O217" s="12" t="n"/>
+      <c r="P217" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="7" t="inlineStr">
@@ -6415,6 +7554,11 @@
       <c r="M218" s="12" t="n"/>
       <c r="N218" s="12" t="n"/>
       <c r="O218" s="12" t="n"/>
+      <c r="P218" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="7" t="inlineStr">
@@ -6442,6 +7586,11 @@
       <c r="M219" s="12" t="n"/>
       <c r="N219" s="12" t="n"/>
       <c r="O219" s="12" t="n"/>
+      <c r="P219" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="7" t="inlineStr">
@@ -6469,6 +7618,11 @@
       <c r="M220" s="12" t="n"/>
       <c r="N220" s="12" t="n"/>
       <c r="O220" s="12" t="n"/>
+      <c r="P220" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="7" t="inlineStr">
@@ -6496,6 +7650,11 @@
       <c r="M221" s="12" t="n"/>
       <c r="N221" s="12" t="n"/>
       <c r="O221" s="12" t="n"/>
+      <c r="P221" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="7" t="inlineStr">
@@ -6523,6 +7682,11 @@
       <c r="M222" s="12" t="n"/>
       <c r="N222" s="12" t="n"/>
       <c r="O222" s="12" t="n"/>
+      <c r="P222" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="7" t="inlineStr">
@@ -6550,6 +7714,11 @@
       <c r="M223" s="12" t="n"/>
       <c r="N223" s="12" t="n"/>
       <c r="O223" s="12" t="n"/>
+      <c r="P223" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="7" t="inlineStr">
@@ -6577,6 +7746,11 @@
       <c r="M224" s="12" t="n"/>
       <c r="N224" s="12" t="n"/>
       <c r="O224" s="12" t="n"/>
+      <c r="P224" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="7" t="inlineStr">
@@ -6604,6 +7778,11 @@
       <c r="M225" s="12" t="n"/>
       <c r="N225" s="12" t="n"/>
       <c r="O225" s="12" t="n"/>
+      <c r="P225" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="7" t="inlineStr">
@@ -6631,6 +7810,11 @@
       <c r="M226" s="12" t="n"/>
       <c r="N226" s="12" t="n"/>
       <c r="O226" s="12" t="n"/>
+      <c r="P226" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="7" t="inlineStr">
@@ -6658,6 +7842,11 @@
       <c r="M227" s="12" t="n"/>
       <c r="N227" s="12" t="n"/>
       <c r="O227" s="12" t="n"/>
+      <c r="P227" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="7" t="inlineStr">
@@ -6685,6 +7874,11 @@
       <c r="M228" s="12" t="n"/>
       <c r="N228" s="12" t="n"/>
       <c r="O228" s="12" t="n"/>
+      <c r="P228" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="7" t="inlineStr">
@@ -6712,6 +7906,11 @@
       <c r="M229" s="12" t="n"/>
       <c r="N229" s="12" t="n"/>
       <c r="O229" s="12" t="n"/>
+      <c r="P229" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="7" t="inlineStr">
@@ -6739,6 +7938,11 @@
       <c r="M230" s="12" t="n"/>
       <c r="N230" s="12" t="n"/>
       <c r="O230" s="12" t="n"/>
+      <c r="P230" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="7" t="inlineStr">
@@ -6766,6 +7970,11 @@
       <c r="M231" s="12" t="n"/>
       <c r="N231" s="12" t="n"/>
       <c r="O231" s="12" t="n"/>
+      <c r="P231" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="7" t="inlineStr">
@@ -6793,6 +8002,11 @@
       <c r="M232" s="12" t="n"/>
       <c r="N232" s="12" t="n"/>
       <c r="O232" s="12" t="n"/>
+      <c r="P232" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="7" t="inlineStr">
@@ -6820,6 +8034,11 @@
       <c r="M233" s="12" t="n"/>
       <c r="N233" s="12" t="n"/>
       <c r="O233" s="12" t="n"/>
+      <c r="P233" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="7" t="inlineStr">
@@ -6847,6 +8066,11 @@
       <c r="M234" s="12" t="n"/>
       <c r="N234" s="12" t="n"/>
       <c r="O234" s="12" t="n"/>
+      <c r="P234" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="7" t="inlineStr">
@@ -6874,6 +8098,11 @@
       <c r="M235" s="12" t="n"/>
       <c r="N235" s="12" t="n"/>
       <c r="O235" s="12" t="n"/>
+      <c r="P235" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="7" t="inlineStr">
@@ -6901,6 +8130,11 @@
       <c r="M236" s="12" t="n"/>
       <c r="N236" s="12" t="n"/>
       <c r="O236" s="12" t="n"/>
+      <c r="P236" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="7" t="inlineStr">
@@ -6928,6 +8162,11 @@
       <c r="M237" s="12" t="n"/>
       <c r="N237" s="12" t="n"/>
       <c r="O237" s="12" t="n"/>
+      <c r="P237" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="7" t="inlineStr">
@@ -6955,6 +8194,11 @@
       <c r="M238" s="12" t="n"/>
       <c r="N238" s="12" t="n"/>
       <c r="O238" s="12" t="n"/>
+      <c r="P238" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="7" t="inlineStr">
@@ -6982,6 +8226,11 @@
       <c r="M239" s="12" t="n"/>
       <c r="N239" s="12" t="n"/>
       <c r="O239" s="12" t="n"/>
+      <c r="P239" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="7" t="inlineStr">
@@ -7009,6 +8258,11 @@
       <c r="M240" s="12" t="n"/>
       <c r="N240" s="12" t="n"/>
       <c r="O240" s="12" t="n"/>
+      <c r="P240" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="7" t="inlineStr">
@@ -7036,6 +8290,11 @@
       <c r="M241" s="12" t="n"/>
       <c r="N241" s="12" t="n"/>
       <c r="O241" s="12" t="n"/>
+      <c r="P241" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="7" t="inlineStr">
@@ -7063,6 +8322,11 @@
       <c r="M242" s="12" t="n"/>
       <c r="N242" s="12" t="n"/>
       <c r="O242" s="12" t="n"/>
+      <c r="P242" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="7" t="inlineStr">
@@ -7090,6 +8354,11 @@
       <c r="M243" s="12" t="n"/>
       <c r="N243" s="12" t="n"/>
       <c r="O243" s="12" t="n"/>
+      <c r="P243" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="7" t="inlineStr">
@@ -7117,6 +8386,11 @@
       <c r="M244" s="12" t="n"/>
       <c r="N244" s="12" t="n"/>
       <c r="O244" s="12" t="n"/>
+      <c r="P244" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="7" t="inlineStr">
@@ -7144,6 +8418,11 @@
       <c r="M245" s="12" t="n"/>
       <c r="N245" s="12" t="n"/>
       <c r="O245" s="12" t="n"/>
+      <c r="P245" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="7" t="inlineStr">
@@ -7171,6 +8450,11 @@
       <c r="M246" s="12" t="n"/>
       <c r="N246" s="12" t="n"/>
       <c r="O246" s="12" t="n"/>
+      <c r="P246" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="7" t="inlineStr">
@@ -7198,6 +8482,11 @@
       <c r="M247" s="12" t="n"/>
       <c r="N247" s="12" t="n"/>
       <c r="O247" s="12" t="n"/>
+      <c r="P247" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="7" t="inlineStr">
@@ -7225,6 +8514,11 @@
       <c r="M248" s="12" t="n"/>
       <c r="N248" s="12" t="n"/>
       <c r="O248" s="12" t="n"/>
+      <c r="P248" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="7" t="inlineStr">
@@ -7252,6 +8546,11 @@
       <c r="M249" s="12" t="n"/>
       <c r="N249" s="12" t="n"/>
       <c r="O249" s="12" t="n"/>
+      <c r="P249" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="7" t="inlineStr">
@@ -7279,6 +8578,11 @@
       <c r="M250" s="12" t="n"/>
       <c r="N250" s="12" t="n"/>
       <c r="O250" s="12" t="n"/>
+      <c r="P250" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="7" t="inlineStr">
@@ -7306,6 +8610,11 @@
       <c r="M251" s="12" t="n"/>
       <c r="N251" s="12" t="n"/>
       <c r="O251" s="12" t="n"/>
+      <c r="P251" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="7" t="inlineStr">
@@ -7333,6 +8642,11 @@
       <c r="M252" s="12" t="n"/>
       <c r="N252" s="12" t="n"/>
       <c r="O252" s="12" t="n"/>
+      <c r="P252" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="7" t="inlineStr">
@@ -7360,6 +8674,11 @@
       <c r="M253" s="12" t="n"/>
       <c r="N253" s="12" t="n"/>
       <c r="O253" s="12" t="n"/>
+      <c r="P253" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="7" t="inlineStr">
@@ -7387,6 +8706,11 @@
       <c r="M254" s="12" t="n"/>
       <c r="N254" s="12" t="n"/>
       <c r="O254" s="12" t="n"/>
+      <c r="P254" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="7" t="inlineStr">
@@ -7414,6 +8738,11 @@
       <c r="M255" s="12" t="n"/>
       <c r="N255" s="12" t="n"/>
       <c r="O255" s="12" t="n"/>
+      <c r="P255" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="7" t="inlineStr">
@@ -7441,6 +8770,11 @@
       <c r="M256" s="12" t="n"/>
       <c r="N256" s="12" t="n"/>
       <c r="O256" s="12" t="n"/>
+      <c r="P256" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="7" t="inlineStr">
@@ -7468,6 +8802,11 @@
       <c r="M257" s="12" t="n"/>
       <c r="N257" s="12" t="n"/>
       <c r="O257" s="12" t="n"/>
+      <c r="P257" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="7" t="inlineStr">
@@ -7495,6 +8834,11 @@
       <c r="M258" s="12" t="n"/>
       <c r="N258" s="12" t="n"/>
       <c r="O258" s="12" t="n"/>
+      <c r="P258" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="7" t="inlineStr">
@@ -7522,6 +8866,11 @@
       <c r="M259" s="12" t="n"/>
       <c r="N259" s="12" t="n"/>
       <c r="O259" s="12" t="n"/>
+      <c r="P259" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="7" t="inlineStr">
@@ -7549,6 +8898,11 @@
       <c r="M260" s="12" t="n"/>
       <c r="N260" s="12" t="n"/>
       <c r="O260" s="12" t="n"/>
+      <c r="P260" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="7" t="inlineStr">
@@ -7576,6 +8930,11 @@
       <c r="M261" s="12" t="n"/>
       <c r="N261" s="12" t="n"/>
       <c r="O261" s="12" t="n"/>
+      <c r="P261" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="7" t="inlineStr">
@@ -7603,6 +8962,11 @@
       <c r="M262" s="12" t="n"/>
       <c r="N262" s="12" t="n"/>
       <c r="O262" s="12" t="n"/>
+      <c r="P262" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="7" t="inlineStr">
@@ -7630,6 +8994,11 @@
       <c r="M263" s="12" t="n"/>
       <c r="N263" s="12" t="n"/>
       <c r="O263" s="12" t="n"/>
+      <c r="P263" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="7" t="inlineStr">
@@ -7657,6 +9026,11 @@
       <c r="M264" s="12" t="n"/>
       <c r="N264" s="12" t="n"/>
       <c r="O264" s="12" t="n"/>
+      <c r="P264" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="7" t="inlineStr">
@@ -7684,6 +9058,11 @@
       <c r="M265" s="12" t="n"/>
       <c r="N265" s="12" t="n"/>
       <c r="O265" s="12" t="n"/>
+      <c r="P265" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="7" t="inlineStr">
@@ -7711,6 +9090,11 @@
       <c r="M266" s="12" t="n"/>
       <c r="N266" s="12" t="n"/>
       <c r="O266" s="12" t="n"/>
+      <c r="P266" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="7" t="inlineStr">
@@ -7738,6 +9122,11 @@
       <c r="M267" s="12" t="n"/>
       <c r="N267" s="12" t="n"/>
       <c r="O267" s="12" t="n"/>
+      <c r="P267" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="7" t="inlineStr">
@@ -7765,6 +9154,11 @@
       <c r="M268" s="12" t="n"/>
       <c r="N268" s="12" t="n"/>
       <c r="O268" s="12" t="n"/>
+      <c r="P268" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="7" t="inlineStr">
@@ -7792,6 +9186,11 @@
       <c r="M269" s="12" t="n"/>
       <c r="N269" s="12" t="n"/>
       <c r="O269" s="12" t="n"/>
+      <c r="P269" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="7" t="inlineStr">
@@ -7819,6 +9218,11 @@
       <c r="M270" s="12" t="n"/>
       <c r="N270" s="12" t="n"/>
       <c r="O270" s="12" t="n"/>
+      <c r="P270" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="7" t="inlineStr">
@@ -7846,6 +9250,11 @@
       <c r="M271" s="12" t="n"/>
       <c r="N271" s="12" t="n"/>
       <c r="O271" s="12" t="n"/>
+      <c r="P271" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="7" t="inlineStr">
@@ -7873,6 +9282,11 @@
       <c r="M272" s="12" t="n"/>
       <c r="N272" s="12" t="n"/>
       <c r="O272" s="12" t="n"/>
+      <c r="P272" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="7" t="inlineStr">
@@ -7900,6 +9314,11 @@
       <c r="M273" s="12" t="n"/>
       <c r="N273" s="12" t="n"/>
       <c r="O273" s="12" t="n"/>
+      <c r="P273" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="7" t="inlineStr">
@@ -7927,6 +9346,11 @@
       <c r="M274" s="12" t="n"/>
       <c r="N274" s="12" t="n"/>
       <c r="O274" s="12" t="n"/>
+      <c r="P274" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="7" t="inlineStr">
@@ -7954,6 +9378,11 @@
       <c r="M275" s="12" t="n"/>
       <c r="N275" s="12" t="n"/>
       <c r="O275" s="12" t="n"/>
+      <c r="P275" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="7" t="inlineStr">
@@ -7981,6 +9410,11 @@
       <c r="M276" s="12" t="n"/>
       <c r="N276" s="12" t="n"/>
       <c r="O276" s="12" t="n"/>
+      <c r="P276" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="7" t="inlineStr">
@@ -8008,6 +9442,11 @@
       <c r="M277" s="12" t="n"/>
       <c r="N277" s="12" t="n"/>
       <c r="O277" s="12" t="n"/>
+      <c r="P277" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="7" t="inlineStr">
@@ -8035,6 +9474,11 @@
       <c r="M278" s="12" t="n"/>
       <c r="N278" s="12" t="n"/>
       <c r="O278" s="12" t="n"/>
+      <c r="P278" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="7" t="inlineStr">
@@ -8062,6 +9506,11 @@
       <c r="M279" s="12" t="n"/>
       <c r="N279" s="12" t="n"/>
       <c r="O279" s="12" t="n"/>
+      <c r="P279" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="280">
       <c r="A280" s="7" t="inlineStr">
@@ -8089,6 +9538,11 @@
       <c r="M280" s="12" t="n"/>
       <c r="N280" s="12" t="n"/>
       <c r="O280" s="12" t="n"/>
+      <c r="P280" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" s="7" t="inlineStr">
@@ -8116,6 +9570,11 @@
       <c r="M281" s="12" t="n"/>
       <c r="N281" s="12" t="n"/>
       <c r="O281" s="12" t="n"/>
+      <c r="P281" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="282">
       <c r="A282" s="7" t="inlineStr">
@@ -8143,6 +9602,11 @@
       <c r="M282" s="12" t="n"/>
       <c r="N282" s="12" t="n"/>
       <c r="O282" s="12" t="n"/>
+      <c r="P282" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="283">
       <c r="A283" s="7" t="inlineStr">
@@ -8170,6 +9634,11 @@
       <c r="M283" s="12" t="n"/>
       <c r="N283" s="12" t="n"/>
       <c r="O283" s="12" t="n"/>
+      <c r="P283" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="284">
       <c r="A284" s="7" t="inlineStr">
@@ -8197,6 +9666,11 @@
       <c r="M284" s="12" t="n"/>
       <c r="N284" s="12" t="n"/>
       <c r="O284" s="12" t="n"/>
+      <c r="P284" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="285">
       <c r="A285" s="7" t="inlineStr">
@@ -8224,6 +9698,11 @@
       <c r="M285" s="12" t="n"/>
       <c r="N285" s="12" t="n"/>
       <c r="O285" s="12" t="n"/>
+      <c r="P285" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="286">
       <c r="A286" s="7" t="inlineStr">
@@ -8251,6 +9730,11 @@
       <c r="M286" s="12" t="n"/>
       <c r="N286" s="12" t="n"/>
       <c r="O286" s="12" t="n"/>
+      <c r="P286" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="7" t="inlineStr">
@@ -8278,6 +9762,11 @@
       <c r="M287" s="12" t="n"/>
       <c r="N287" s="12" t="n"/>
       <c r="O287" s="12" t="n"/>
+      <c r="P287" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="7" t="inlineStr">
@@ -8305,6 +9794,11 @@
       <c r="M288" s="12" t="n"/>
       <c r="N288" s="12" t="n"/>
       <c r="O288" s="12" t="n"/>
+      <c r="P288" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="289">
       <c r="A289" s="7" t="inlineStr">
@@ -8332,6 +9826,11 @@
       <c r="M289" s="12" t="n"/>
       <c r="N289" s="12" t="n"/>
       <c r="O289" s="12" t="n"/>
+      <c r="P289" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" s="7" t="inlineStr">
@@ -8359,6 +9858,11 @@
       <c r="M290" s="12" t="n"/>
       <c r="N290" s="12" t="n"/>
       <c r="O290" s="12" t="n"/>
+      <c r="P290" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" s="7" t="inlineStr">
@@ -8386,6 +9890,11 @@
       <c r="M291" s="12" t="n"/>
       <c r="N291" s="12" t="n"/>
       <c r="O291" s="12" t="n"/>
+      <c r="P291" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="292">
       <c r="A292" s="7" t="inlineStr">
@@ -8413,6 +9922,11 @@
       <c r="M292" s="12" t="n"/>
       <c r="N292" s="12" t="n"/>
       <c r="O292" s="12" t="n"/>
+      <c r="P292" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="293">
       <c r="A293" s="7" t="inlineStr">
@@ -8440,6 +9954,11 @@
       <c r="M293" s="12" t="n"/>
       <c r="N293" s="12" t="n"/>
       <c r="O293" s="12" t="n"/>
+      <c r="P293" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="294">
       <c r="A294" s="7" t="inlineStr">
@@ -8467,6 +9986,11 @@
       <c r="M294" s="12" t="n"/>
       <c r="N294" s="12" t="n"/>
       <c r="O294" s="12" t="n"/>
+      <c r="P294" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="295">
       <c r="A295" s="7" t="inlineStr">
@@ -8494,6 +10018,11 @@
       <c r="M295" s="12" t="n"/>
       <c r="N295" s="12" t="n"/>
       <c r="O295" s="12" t="n"/>
+      <c r="P295" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="296">
       <c r="A296" s="7" t="inlineStr">
@@ -8521,6 +10050,11 @@
       <c r="M296" s="12" t="n"/>
       <c r="N296" s="12" t="n"/>
       <c r="O296" s="12" t="n"/>
+      <c r="P296" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="297">
       <c r="A297" s="7" t="inlineStr">
@@ -8548,6 +10082,11 @@
       <c r="M297" s="12" t="n"/>
       <c r="N297" s="12" t="n"/>
       <c r="O297" s="12" t="n"/>
+      <c r="P297" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="298">
       <c r="A298" s="7" t="inlineStr">
@@ -8575,6 +10114,11 @@
       <c r="M298" s="12" t="n"/>
       <c r="N298" s="12" t="n"/>
       <c r="O298" s="12" t="n"/>
+      <c r="P298" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" s="7" t="inlineStr">
@@ -8602,6 +10146,11 @@
       <c r="M299" s="12" t="n"/>
       <c r="N299" s="12" t="n"/>
       <c r="O299" s="12" t="n"/>
+      <c r="P299" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="300">
       <c r="A300" s="7" t="inlineStr">
@@ -8629,6 +10178,11 @@
       <c r="M300" s="12" t="n"/>
       <c r="N300" s="12" t="n"/>
       <c r="O300" s="12" t="n"/>
+      <c r="P300" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="301">
       <c r="A301" s="7" t="inlineStr">
@@ -8656,6 +10210,11 @@
       <c r="M301" s="12" t="n"/>
       <c r="N301" s="12" t="n"/>
       <c r="O301" s="12" t="n"/>
+      <c r="P301" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="302">
       <c r="A302" s="7" t="inlineStr">
@@ -8683,6 +10242,11 @@
       <c r="M302" s="12" t="n"/>
       <c r="N302" s="12" t="n"/>
       <c r="O302" s="12" t="n"/>
+      <c r="P302" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="303">
       <c r="A303" s="7" t="inlineStr">
@@ -8710,6 +10274,11 @@
       <c r="M303" s="12" t="n"/>
       <c r="N303" s="12" t="n"/>
       <c r="O303" s="12" t="n"/>
+      <c r="P303" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="304">
       <c r="A304" s="7" t="inlineStr">
@@ -8737,6 +10306,11 @@
       <c r="M304" s="12" t="n"/>
       <c r="N304" s="12" t="n"/>
       <c r="O304" s="12" t="n"/>
+      <c r="P304" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="305">
       <c r="A305" s="7" t="inlineStr">
@@ -8764,6 +10338,11 @@
       <c r="M305" s="12" t="n"/>
       <c r="N305" s="12" t="n"/>
       <c r="O305" s="12" t="n"/>
+      <c r="P305" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="306">
       <c r="A306" s="7" t="inlineStr">
@@ -8791,6 +10370,11 @@
       <c r="M306" s="12" t="n"/>
       <c r="N306" s="12" t="n"/>
       <c r="O306" s="12" t="n"/>
+      <c r="P306" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="307">
       <c r="A307" s="7" t="inlineStr">
@@ -8818,6 +10402,11 @@
       <c r="M307" s="12" t="n"/>
       <c r="N307" s="12" t="n"/>
       <c r="O307" s="12" t="n"/>
+      <c r="P307" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="308">
       <c r="A308" s="7" t="inlineStr">
@@ -8845,6 +10434,11 @@
       <c r="M308" s="12" t="n"/>
       <c r="N308" s="12" t="n"/>
       <c r="O308" s="12" t="n"/>
+      <c r="P308" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="309">
       <c r="A309" s="7" t="inlineStr">
@@ -8872,6 +10466,11 @@
       <c r="M309" s="12" t="n"/>
       <c r="N309" s="12" t="n"/>
       <c r="O309" s="12" t="n"/>
+      <c r="P309" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="310">
       <c r="A310" s="7" t="inlineStr">
@@ -8899,6 +10498,11 @@
       <c r="M310" s="12" t="n"/>
       <c r="N310" s="12" t="n"/>
       <c r="O310" s="12" t="n"/>
+      <c r="P310" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="311">
       <c r="A311" s="7" t="inlineStr">
@@ -8926,6 +10530,11 @@
       <c r="M311" s="12" t="n"/>
       <c r="N311" s="12" t="n"/>
       <c r="O311" s="12" t="n"/>
+      <c r="P311" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="312">
       <c r="A312" s="7" t="inlineStr">
@@ -8953,6 +10562,11 @@
       <c r="M312" s="12" t="n"/>
       <c r="N312" s="12" t="n"/>
       <c r="O312" s="12" t="n"/>
+      <c r="P312" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="313">
       <c r="A313" s="7" t="inlineStr">
@@ -8980,6 +10594,11 @@
       <c r="M313" s="12" t="n"/>
       <c r="N313" s="12" t="n"/>
       <c r="O313" s="12" t="n"/>
+      <c r="P313" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="314">
       <c r="A314" s="7" t="inlineStr">
@@ -9007,6 +10626,11 @@
       <c r="M314" s="12" t="n"/>
       <c r="N314" s="12" t="n"/>
       <c r="O314" s="12" t="n"/>
+      <c r="P314" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="315">
       <c r="A315" s="7" t="inlineStr">
@@ -9034,6 +10658,11 @@
       <c r="M315" s="12" t="n"/>
       <c r="N315" s="12" t="n"/>
       <c r="O315" s="12" t="n"/>
+      <c r="P315" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="316">
       <c r="A316" s="7" t="inlineStr">
@@ -9061,6 +10690,11 @@
       <c r="M316" s="12" t="n"/>
       <c r="N316" s="12" t="n"/>
       <c r="O316" s="12" t="n"/>
+      <c r="P316" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="317">
       <c r="A317" s="7" t="inlineStr">
@@ -9088,6 +10722,11 @@
       <c r="M317" s="12" t="n"/>
       <c r="N317" s="12" t="n"/>
       <c r="O317" s="12" t="n"/>
+      <c r="P317" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="318">
       <c r="A318" s="7" t="inlineStr">
@@ -9115,6 +10754,11 @@
       <c r="M318" s="12" t="n"/>
       <c r="N318" s="12" t="n"/>
       <c r="O318" s="12" t="n"/>
+      <c r="P318" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="319">
       <c r="A319" s="7" t="inlineStr">
@@ -9142,6 +10786,11 @@
       <c r="M319" s="12" t="n"/>
       <c r="N319" s="12" t="n"/>
       <c r="O319" s="12" t="n"/>
+      <c r="P319" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="320">
       <c r="A320" s="7" t="inlineStr">
@@ -9169,6 +10818,11 @@
       <c r="M320" s="12" t="n"/>
       <c r="N320" s="12" t="n"/>
       <c r="O320" s="12" t="n"/>
+      <c r="P320" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="321">
       <c r="A321" s="7" t="inlineStr">
@@ -9196,6 +10850,11 @@
       <c r="M321" s="12" t="n"/>
       <c r="N321" s="12" t="n"/>
       <c r="O321" s="12" t="n"/>
+      <c r="P321" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="322">
       <c r="A322" s="7" t="inlineStr">
@@ -9223,6 +10882,11 @@
       <c r="M322" s="12" t="n"/>
       <c r="N322" s="12" t="n"/>
       <c r="O322" s="12" t="n"/>
+      <c r="P322" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="323">
       <c r="A323" s="7" t="inlineStr">
@@ -9250,6 +10914,11 @@
       <c r="M323" s="12" t="n"/>
       <c r="N323" s="12" t="n"/>
       <c r="O323" s="12" t="n"/>
+      <c r="P323" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="324">
       <c r="A324" s="7" t="inlineStr">
@@ -9277,6 +10946,11 @@
       <c r="M324" s="12" t="n"/>
       <c r="N324" s="12" t="n"/>
       <c r="O324" s="12" t="n"/>
+      <c r="P324" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="325">
       <c r="A325" s="7" t="inlineStr">
@@ -9304,6 +10978,11 @@
       <c r="M325" s="12" t="n"/>
       <c r="N325" s="12" t="n"/>
       <c r="O325" s="12" t="n"/>
+      <c r="P325" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="326">
       <c r="A326" s="7" t="inlineStr">
@@ -9331,6 +11010,11 @@
       <c r="M326" s="12" t="n"/>
       <c r="N326" s="12" t="n"/>
       <c r="O326" s="12" t="n"/>
+      <c r="P326" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="327">
       <c r="A327" s="7" t="inlineStr">
@@ -9358,6 +11042,11 @@
       <c r="M327" s="12" t="n"/>
       <c r="N327" s="12" t="n"/>
       <c r="O327" s="12" t="n"/>
+      <c r="P327" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="328">
       <c r="A328" s="7" t="inlineStr">
@@ -9385,6 +11074,11 @@
       <c r="M328" s="12" t="n"/>
       <c r="N328" s="12" t="n"/>
       <c r="O328" s="12" t="n"/>
+      <c r="P328" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="329">
       <c r="A329" s="7" t="inlineStr">
@@ -9412,6 +11106,11 @@
       <c r="M329" s="12" t="n"/>
       <c r="N329" s="12" t="n"/>
       <c r="O329" s="12" t="n"/>
+      <c r="P329" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="330">
       <c r="A330" s="7" t="inlineStr">
@@ -9439,6 +11138,11 @@
       <c r="M330" s="12" t="n"/>
       <c r="N330" s="12" t="n"/>
       <c r="O330" s="12" t="n"/>
+      <c r="P330" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="331">
       <c r="A331" s="7" t="inlineStr">
@@ -9466,6 +11170,11 @@
       <c r="M331" s="12" t="n"/>
       <c r="N331" s="12" t="n"/>
       <c r="O331" s="12" t="n"/>
+      <c r="P331" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="332">
       <c r="A332" s="7" t="inlineStr">
@@ -9493,6 +11202,11 @@
       <c r="M332" s="12" t="n"/>
       <c r="N332" s="12" t="n"/>
       <c r="O332" s="12" t="n"/>
+      <c r="P332" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="333">
       <c r="A333" s="7" t="inlineStr">
@@ -9520,6 +11234,11 @@
       <c r="M333" s="12" t="n"/>
       <c r="N333" s="12" t="n"/>
       <c r="O333" s="12" t="n"/>
+      <c r="P333" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="334">
       <c r="A334" s="7" t="inlineStr">
@@ -9547,6 +11266,11 @@
       <c r="M334" s="12" t="n"/>
       <c r="N334" s="12" t="n"/>
       <c r="O334" s="12" t="n"/>
+      <c r="P334" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="335">
       <c r="A335" s="7" t="inlineStr">
@@ -9574,6 +11298,11 @@
       <c r="M335" s="12" t="n"/>
       <c r="N335" s="12" t="n"/>
       <c r="O335" s="12" t="n"/>
+      <c r="P335" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="336">
       <c r="A336" s="7" t="inlineStr">
@@ -9601,6 +11330,11 @@
       <c r="M336" s="12" t="n"/>
       <c r="N336" s="12" t="n"/>
       <c r="O336" s="12" t="n"/>
+      <c r="P336" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="337">
       <c r="A337" s="7" t="inlineStr">
@@ -9628,6 +11362,11 @@
       <c r="M337" s="12" t="n"/>
       <c r="N337" s="12" t="n"/>
       <c r="O337" s="12" t="n"/>
+      <c r="P337" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="338">
       <c r="A338" s="7" t="inlineStr">
@@ -9655,6 +11394,11 @@
       <c r="M338" s="12" t="n"/>
       <c r="N338" s="12" t="n"/>
       <c r="O338" s="12" t="n"/>
+      <c r="P338" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="339">
       <c r="A339" s="7" t="inlineStr">
@@ -9682,6 +11426,11 @@
       <c r="M339" s="12" t="n"/>
       <c r="N339" s="12" t="n"/>
       <c r="O339" s="12" t="n"/>
+      <c r="P339" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="340">
       <c r="A340" s="7" t="inlineStr">
@@ -9709,6 +11458,11 @@
       <c r="M340" s="12" t="n"/>
       <c r="N340" s="12" t="n"/>
       <c r="O340" s="12" t="n"/>
+      <c r="P340" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="7" t="inlineStr">
@@ -9736,6 +11490,11 @@
       <c r="M341" s="12" t="n"/>
       <c r="N341" s="12" t="n"/>
       <c r="O341" s="12" t="n"/>
+      <c r="P341" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="342">
       <c r="A342" s="7" t="inlineStr">
@@ -9763,6 +11522,11 @@
       <c r="M342" s="12" t="n"/>
       <c r="N342" s="12" t="n"/>
       <c r="O342" s="12" t="n"/>
+      <c r="P342" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="343">
       <c r="A343" s="7" t="inlineStr">
@@ -9790,6 +11554,11 @@
       <c r="M343" s="12" t="n"/>
       <c r="N343" s="12" t="n"/>
       <c r="O343" s="12" t="n"/>
+      <c r="P343" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="344">
       <c r="A344" s="7" t="inlineStr">
@@ -9817,6 +11586,11 @@
       <c r="M344" s="12" t="n"/>
       <c r="N344" s="12" t="n"/>
       <c r="O344" s="12" t="n"/>
+      <c r="P344" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="345">
       <c r="A345" s="7" t="inlineStr">
@@ -9844,6 +11618,11 @@
       <c r="M345" s="12" t="n"/>
       <c r="N345" s="12" t="n"/>
       <c r="O345" s="12" t="n"/>
+      <c r="P345" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="346">
       <c r="A346" s="7" t="inlineStr">
@@ -9871,6 +11650,11 @@
       <c r="M346" s="12" t="n"/>
       <c r="N346" s="12" t="n"/>
       <c r="O346" s="12" t="n"/>
+      <c r="P346" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" s="7" t="inlineStr">
@@ -9898,6 +11682,11 @@
       <c r="M347" s="12" t="n"/>
       <c r="N347" s="12" t="n"/>
       <c r="O347" s="12" t="n"/>
+      <c r="P347" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="348">
       <c r="A348" s="7" t="inlineStr">
@@ -9925,6 +11714,11 @@
       <c r="M348" s="12" t="n"/>
       <c r="N348" s="12" t="n"/>
       <c r="O348" s="12" t="n"/>
+      <c r="P348" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="349">
       <c r="A349" s="7" t="inlineStr">
@@ -9952,6 +11746,11 @@
       <c r="M349" s="12" t="n"/>
       <c r="N349" s="12" t="n"/>
       <c r="O349" s="12" t="n"/>
+      <c r="P349" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="350">
       <c r="A350" s="7" t="inlineStr">
@@ -9979,6 +11778,11 @@
       <c r="M350" s="12" t="n"/>
       <c r="N350" s="12" t="n"/>
       <c r="O350" s="12" t="n"/>
+      <c r="P350" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="351">
       <c r="A351" s="7" t="inlineStr">
@@ -10006,6 +11810,11 @@
       <c r="M351" s="12" t="n"/>
       <c r="N351" s="12" t="n"/>
       <c r="O351" s="12" t="n"/>
+      <c r="P351" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="352">
       <c r="A352" s="7" t="inlineStr">
@@ -10033,6 +11842,11 @@
       <c r="M352" s="12" t="n"/>
       <c r="N352" s="12" t="n"/>
       <c r="O352" s="12" t="n"/>
+      <c r="P352" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="353">
       <c r="A353" s="7" t="inlineStr">
@@ -10060,6 +11874,11 @@
       <c r="M353" s="12" t="n"/>
       <c r="N353" s="12" t="n"/>
       <c r="O353" s="12" t="n"/>
+      <c r="P353" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="354">
       <c r="A354" s="7" t="inlineStr">
@@ -10087,6 +11906,11 @@
       <c r="M354" s="12" t="n"/>
       <c r="N354" s="12" t="n"/>
       <c r="O354" s="12" t="n"/>
+      <c r="P354" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="355">
       <c r="A355" s="7" t="inlineStr">
@@ -10114,6 +11938,11 @@
       <c r="M355" s="12" t="n"/>
       <c r="N355" s="12" t="n"/>
       <c r="O355" s="12" t="n"/>
+      <c r="P355" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="356">
       <c r="A356" s="7" t="inlineStr">
@@ -10141,6 +11970,11 @@
       <c r="M356" s="12" t="n"/>
       <c r="N356" s="12" t="n"/>
       <c r="O356" s="12" t="n"/>
+      <c r="P356" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="357">
       <c r="A357" s="7" t="inlineStr">
@@ -10168,6 +12002,11 @@
       <c r="M357" s="12" t="n"/>
       <c r="N357" s="12" t="n"/>
       <c r="O357" s="12" t="n"/>
+      <c r="P357" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="358">
       <c r="A358" s="7" t="inlineStr">
@@ -10195,6 +12034,11 @@
       <c r="M358" s="12" t="n"/>
       <c r="N358" s="12" t="n"/>
       <c r="O358" s="12" t="n"/>
+      <c r="P358" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="359">
       <c r="A359" s="7" t="inlineStr">
@@ -10222,6 +12066,11 @@
       <c r="M359" s="12" t="n"/>
       <c r="N359" s="12" t="n"/>
       <c r="O359" s="12" t="n"/>
+      <c r="P359" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="360">
       <c r="A360" s="7" t="inlineStr">
@@ -10249,6 +12098,11 @@
       <c r="M360" s="12" t="n"/>
       <c r="N360" s="12" t="n"/>
       <c r="O360" s="12" t="n"/>
+      <c r="P360" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" s="7" t="inlineStr">
@@ -10276,6 +12130,11 @@
       <c r="M361" s="12" t="n"/>
       <c r="N361" s="12" t="n"/>
       <c r="O361" s="12" t="n"/>
+      <c r="P361" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="362">
       <c r="A362" s="7" t="inlineStr">
@@ -10303,6 +12162,11 @@
       <c r="M362" s="12" t="n"/>
       <c r="N362" s="12" t="n"/>
       <c r="O362" s="12" t="n"/>
+      <c r="P362" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="363">
       <c r="A363" s="7" t="inlineStr">
@@ -10330,6 +12194,11 @@
       <c r="M363" s="12" t="n"/>
       <c r="N363" s="12" t="n"/>
       <c r="O363" s="12" t="n"/>
+      <c r="P363" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="364">
       <c r="A364" s="7" t="inlineStr">
@@ -10357,6 +12226,11 @@
       <c r="M364" s="12" t="n"/>
       <c r="N364" s="12" t="n"/>
       <c r="O364" s="12" t="n"/>
+      <c r="P364" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" s="7" t="inlineStr">
@@ -10384,6 +12258,11 @@
       <c r="M365" s="12" t="n"/>
       <c r="N365" s="12" t="n"/>
       <c r="O365" s="12" t="n"/>
+      <c r="P365" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="366">
       <c r="A366" s="7" t="inlineStr">
@@ -10411,6 +12290,11 @@
       <c r="M366" s="12" t="n"/>
       <c r="N366" s="12" t="n"/>
       <c r="O366" s="12" t="n"/>
+      <c r="P366" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="367">
       <c r="A367" s="7" t="inlineStr">
@@ -10438,6 +12322,11 @@
       <c r="M367" s="12" t="n"/>
       <c r="N367" s="12" t="n"/>
       <c r="O367" s="12" t="n"/>
+      <c r="P367" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="368">
       <c r="A368" s="7" t="inlineStr">
@@ -10465,6 +12354,11 @@
       <c r="M368" s="12" t="n"/>
       <c r="N368" s="12" t="n"/>
       <c r="O368" s="12" t="n"/>
+      <c r="P368" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="369">
       <c r="A369" s="7" t="inlineStr">
@@ -10492,6 +12386,11 @@
       <c r="M369" s="12" t="n"/>
       <c r="N369" s="12" t="n"/>
       <c r="O369" s="12" t="n"/>
+      <c r="P369" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="370">
       <c r="A370" s="7" t="inlineStr">
@@ -10519,6 +12418,11 @@
       <c r="M370" s="12" t="n"/>
       <c r="N370" s="12" t="n"/>
       <c r="O370" s="12" t="n"/>
+      <c r="P370" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="7" t="inlineStr">
@@ -10546,6 +12450,11 @@
       <c r="M371" s="12" t="n"/>
       <c r="N371" s="12" t="n"/>
       <c r="O371" s="12" t="n"/>
+      <c r="P371" s="35" t="inlineStr">
+        <is>
+          <t>Optimize</t>
+        </is>
+      </c>
     </row>
     <row r="372">
       <c r="A372" s="7" t="inlineStr">
@@ -10573,6 +12482,11 @@
       <c r="M372" s="12" t="n"/>
       <c r="N372" s="12" t="n"/>
       <c r="O372" s="12" t="n"/>
+      <c r="P372" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="373">
       <c r="A373" s="7" t="inlineStr">
@@ -10600,6 +12514,11 @@
       <c r="M373" s="12" t="n"/>
       <c r="N373" s="12" t="n"/>
       <c r="O373" s="12" t="n"/>
+      <c r="P373" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="374">
       <c r="A374" s="7" t="inlineStr">
@@ -10627,6 +12546,11 @@
       <c r="M374" s="12" t="n"/>
       <c r="N374" s="12" t="n"/>
       <c r="O374" s="12" t="n"/>
+      <c r="P374" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="375">
       <c r="A375" s="7" t="inlineStr">
@@ -10654,6 +12578,11 @@
       <c r="M375" s="12" t="n"/>
       <c r="N375" s="12" t="n"/>
       <c r="O375" s="12" t="n"/>
+      <c r="P375" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" s="7" t="inlineStr">
@@ -10681,6 +12610,11 @@
       <c r="M376" s="12" t="n"/>
       <c r="N376" s="12" t="n"/>
       <c r="O376" s="12" t="n"/>
+      <c r="P376" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="377">
       <c r="A377" s="7" t="inlineStr">
@@ -10708,6 +12642,11 @@
       <c r="M377" s="12" t="n"/>
       <c r="N377" s="12" t="n"/>
       <c r="O377" s="12" t="n"/>
+      <c r="P377" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="378">
       <c r="A378" s="7" t="inlineStr">
@@ -10735,6 +12674,11 @@
       <c r="M378" s="12" t="n"/>
       <c r="N378" s="12" t="n"/>
       <c r="O378" s="12" t="n"/>
+      <c r="P378" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="379">
       <c r="A379" s="7" t="inlineStr">
@@ -10762,6 +12706,11 @@
       <c r="M379" s="12" t="n"/>
       <c r="N379" s="12" t="n"/>
       <c r="O379" s="12" t="n"/>
+      <c r="P379" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="380">
       <c r="A380" s="7" t="inlineStr">
@@ -10789,6 +12738,11 @@
       <c r="M380" s="12" t="n"/>
       <c r="N380" s="12" t="n"/>
       <c r="O380" s="12" t="n"/>
+      <c r="P380" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="381">
       <c r="A381" s="7" t="inlineStr">
@@ -10816,6 +12770,11 @@
       <c r="M381" s="12" t="n"/>
       <c r="N381" s="12" t="n"/>
       <c r="O381" s="12" t="n"/>
+      <c r="P381" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="382">
       <c r="A382" s="7" t="inlineStr">
@@ -10843,6 +12802,11 @@
       <c r="M382" s="12" t="n"/>
       <c r="N382" s="12" t="n"/>
       <c r="O382" s="12" t="n"/>
+      <c r="P382" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="383">
       <c r="A383" s="7" t="inlineStr">
@@ -10870,6 +12834,11 @@
       <c r="M383" s="12" t="n"/>
       <c r="N383" s="12" t="n"/>
       <c r="O383" s="12" t="n"/>
+      <c r="P383" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="384">
       <c r="A384" s="7" t="inlineStr">
@@ -10897,6 +12866,11 @@
       <c r="M384" s="12" t="n"/>
       <c r="N384" s="12" t="n"/>
       <c r="O384" s="12" t="n"/>
+      <c r="P384" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="385">
       <c r="A385" s="7" t="inlineStr">
@@ -10924,6 +12898,11 @@
       <c r="M385" s="12" t="n"/>
       <c r="N385" s="12" t="n"/>
       <c r="O385" s="12" t="n"/>
+      <c r="P385" s="37" t="inlineStr">
+        <is>
+          <t>Terminate</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" s="7" t="inlineStr">
@@ -10951,6 +12930,11 @@
       <c r="M386" s="12" t="n"/>
       <c r="N386" s="12" t="n"/>
       <c r="O386" s="12" t="n"/>
+      <c r="P386" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="387">
       <c r="A387" s="7" t="inlineStr">
@@ -10978,6 +12962,11 @@
       <c r="M387" s="12" t="n"/>
       <c r="N387" s="12" t="n"/>
       <c r="O387" s="12" t="n"/>
+      <c r="P387" s="36" t="inlineStr">
+        <is>
+          <t>Consolidate</t>
+        </is>
+      </c>
     </row>
     <row r="388">
       <c r="A388" s="15" t="n"/>

</xml_diff>